<commit_message>
màj couleur saison 22-23
</commit_message>
<xml_diff>
--- a/doc/template.xlsx
+++ b/doc/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoinejamin/Documents/GitHub/generateur-visuel-match-weekend/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E639FF-91A7-A343-9C7A-9999225460EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7572EE8-21A1-8448-A06F-D3E5C895A18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14860" xr2:uid="{3698F051-6750-8E49-B3AD-A92ADC5F0FF9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>U20F</t>
   </si>
@@ -196,6 +196,15 @@
   </si>
   <si>
     <t>AUTHION</t>
+  </si>
+  <si>
+    <t>15H</t>
+  </si>
+  <si>
+    <t>TOTO</t>
+  </si>
+  <si>
+    <t>MONTAIGNE</t>
   </si>
 </sst>
 </file>
@@ -565,7 +574,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -794,10 +803,18 @@
       <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
amélioration chgt taille et espacement
</commit_message>
<xml_diff>
--- a/doc/template.xlsx
+++ b/doc/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoinejamin/Documents/GitHub/generateur-visuel-match-weekend/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09031105-C5B1-584C-81E7-DA4AC0FC1429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A88B11-A8B7-D345-96F3-9E886DEA937B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9260" yWindow="500" windowWidth="16340" windowHeight="14860" xr2:uid="{3698F051-6750-8E49-B3AD-A92ADC5F0FF9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14860" xr2:uid="{3698F051-6750-8E49-B3AD-A92ADC5F0FF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
   <si>
     <t>U13F</t>
   </si>
@@ -126,127 +124,103 @@
     <t>DIMANCHE</t>
   </si>
   <si>
+    <t>TOURNOI</t>
+  </si>
+  <si>
+    <t>15H</t>
+  </si>
+  <si>
+    <t>20H30</t>
+  </si>
+  <si>
+    <t>17H</t>
+  </si>
+  <si>
     <t>14H</t>
   </si>
   <si>
-    <t>TOURNOI</t>
-  </si>
-  <si>
-    <t>15H</t>
+    <t>BEAUCOUZE</t>
+  </si>
+  <si>
+    <t>DREUX VERNOUILLET</t>
+  </si>
+  <si>
+    <t>DREUX</t>
+  </si>
+  <si>
+    <t>17H00</t>
+  </si>
+  <si>
+    <t>AMBRIERES / MAYENNE</t>
+  </si>
+  <si>
+    <t>AMBRIERES</t>
+  </si>
+  <si>
+    <t>17H30</t>
+  </si>
+  <si>
+    <t>ES SEGRE 1</t>
+  </si>
+  <si>
+    <t>SEGRE</t>
+  </si>
+  <si>
+    <t>MONTREUIL J / AVRILLE</t>
+  </si>
+  <si>
+    <t>ST SEBASTIEN SUD LOIRE HB</t>
+  </si>
+  <si>
+    <t>ST SEBASTIEN</t>
+  </si>
+  <si>
+    <t>16H</t>
+  </si>
+  <si>
+    <t>ASPTT NANTES</t>
   </si>
   <si>
     <t>NANTES</t>
   </si>
   <si>
-    <t>21H</t>
-  </si>
-  <si>
-    <t>ANGERS HARAS</t>
-  </si>
-  <si>
-    <t>20H30</t>
-  </si>
-  <si>
-    <t>JOUE LES TOURS</t>
-  </si>
-  <si>
-    <t>16H00</t>
-  </si>
-  <si>
-    <t>RACC DE NANTES</t>
-  </si>
-  <si>
-    <t>18H30</t>
-  </si>
-  <si>
-    <t>US LAVALLOISE HB</t>
-  </si>
-  <si>
-    <t>14H00</t>
-  </si>
-  <si>
-    <t>ES SEGRE HAUT ANJOU</t>
-  </si>
-  <si>
-    <t>15H45</t>
-  </si>
-  <si>
-    <t>ENTENTE ERDRE ET LOIRE</t>
-  </si>
-  <si>
-    <t>SAINTE LUCE</t>
-  </si>
-  <si>
-    <t>14H45</t>
-  </si>
-  <si>
-    <t>ES AUBANCE</t>
-  </si>
-  <si>
-    <t>EXEMPT</t>
-  </si>
-  <si>
-    <t>10H</t>
-  </si>
-  <si>
-    <t>MONTREUIL JUIGNE</t>
-  </si>
-  <si>
-    <t>US JUVARDEIL</t>
-  </si>
-  <si>
-    <t>10H30</t>
-  </si>
-  <si>
-    <t>CHOLET</t>
-  </si>
-  <si>
-    <t>JEAN MONNET</t>
-  </si>
-  <si>
-    <t>16H45</t>
-  </si>
-  <si>
-    <t>HB ST LUCE SUR LOIRE</t>
-  </si>
-  <si>
-    <t>19H</t>
-  </si>
-  <si>
-    <t>ATLANTIQUE REZE HB 2</t>
-  </si>
-  <si>
-    <t>HB LIGERIEN 2</t>
-  </si>
-  <si>
-    <t>MONTREUIL J / AVRILLE</t>
-  </si>
-  <si>
-    <t>HB LIGERIEN</t>
-  </si>
-  <si>
-    <t>17H45</t>
-  </si>
-  <si>
-    <t>LAETITIA DE NANTES</t>
-  </si>
-  <si>
-    <t>17H</t>
-  </si>
-  <si>
-    <t>LA ROCHE SUR YON VHB</t>
-  </si>
-  <si>
-    <t>13H15</t>
-  </si>
-  <si>
-    <t>ES SEGRE 1</t>
-  </si>
-  <si>
-    <t>SCO / STE GEMMES 1</t>
-  </si>
-  <si>
-    <t>13H</t>
+    <t>AIZENAY</t>
+  </si>
+  <si>
+    <t>ENT FERTOIS-ECV</t>
+  </si>
+  <si>
+    <t>CONNERRE</t>
+  </si>
+  <si>
+    <t>13H30</t>
+  </si>
+  <si>
+    <t>HBC AUTION 1</t>
+  </si>
+  <si>
+    <t>BEAUFORT</t>
+  </si>
+  <si>
+    <t>16H15</t>
+  </si>
+  <si>
+    <t>CS BEAUCOUZE</t>
+  </si>
+  <si>
+    <t>CS LE LION D ANGERS 1</t>
+  </si>
+  <si>
+    <t>LE LION D ANGERS</t>
+  </si>
+  <si>
+    <t>AIZEANY</t>
+  </si>
+  <si>
+    <t>14H30</t>
+  </si>
+  <si>
+    <t>BAUGE</t>
   </si>
 </sst>
 </file>
@@ -616,7 +590,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,13 +627,13 @@
         <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -667,54 +641,30 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -722,16 +672,16 @@
         <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -740,16 +690,16 @@
         <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -759,9 +709,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="1"/>
     </row>
@@ -770,13 +718,13 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>51</v>
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>28</v>
@@ -785,224 +733,192 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="1"/>
+        <v>55</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">

</xml_diff>

<commit_message>
V2 : programme et résultats
Génération d'un programme des matchs
Génération d'un affichage des résultats du weekend
</commit_message>
<xml_diff>
--- a/doc/template.xlsx
+++ b/doc/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoinejamin/Documents/GitHub/generateur-visuel-match-weekend/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A88B11-A8B7-D345-96F3-9E886DEA937B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2CF850-4E56-9343-96BF-C3A4BADD2CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14860" xr2:uid="{3698F051-6750-8E49-B3AD-A92ADC5F0FF9}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>U13F</t>
   </si>
@@ -121,113 +121,95 @@
     <t>LIGERIA</t>
   </si>
   <si>
+    <t>17H</t>
+  </si>
+  <si>
     <t>DIMANCHE</t>
   </si>
   <si>
+    <t>SEGRE</t>
+  </si>
+  <si>
+    <t>19H</t>
+  </si>
+  <si>
+    <t>11H30</t>
+  </si>
+  <si>
+    <t>MONTAIGNE</t>
+  </si>
+  <si>
+    <t>CS LE LION D ANGERS</t>
+  </si>
+  <si>
+    <t>HB LIGERIEN</t>
+  </si>
+  <si>
+    <t>16H30</t>
+  </si>
+  <si>
+    <t>LE FRESNE</t>
+  </si>
+  <si>
+    <t>HBC AUTHION</t>
+  </si>
+  <si>
+    <t>ES AUBANCE</t>
+  </si>
+  <si>
+    <t>MONTREUIL JUIGNE</t>
+  </si>
+  <si>
+    <t>15H30</t>
+  </si>
+  <si>
     <t>TOURNOI</t>
   </si>
   <si>
-    <t>15H</t>
-  </si>
-  <si>
-    <t>20H30</t>
-  </si>
-  <si>
-    <t>17H</t>
-  </si>
-  <si>
-    <t>14H</t>
-  </si>
-  <si>
-    <t>BEAUCOUZE</t>
-  </si>
-  <si>
-    <t>DREUX VERNOUILLET</t>
-  </si>
-  <si>
-    <t>DREUX</t>
-  </si>
-  <si>
-    <t>17H00</t>
-  </si>
-  <si>
-    <t>AMBRIERES / MAYENNE</t>
-  </si>
-  <si>
-    <t>AMBRIERES</t>
+    <t>MONTREUIL J / AVRILLE 1</t>
+  </si>
+  <si>
+    <t>LE LION D ANGERS</t>
   </si>
   <si>
     <t>17H30</t>
   </si>
   <si>
-    <t>ES SEGRE 1</t>
-  </si>
-  <si>
-    <t>SEGRE</t>
-  </si>
-  <si>
-    <t>MONTREUIL J / AVRILLE</t>
-  </si>
-  <si>
-    <t>ST SEBASTIEN SUD LOIRE HB</t>
-  </si>
-  <si>
-    <t>ST SEBASTIEN</t>
-  </si>
-  <si>
-    <t>16H</t>
-  </si>
-  <si>
-    <t>ASPTT NANTES</t>
-  </si>
-  <si>
-    <t>NANTES</t>
-  </si>
-  <si>
-    <t>AIZENAY</t>
-  </si>
-  <si>
-    <t>ENT FERTOIS-ECV</t>
-  </si>
-  <si>
-    <t>CONNERRE</t>
-  </si>
-  <si>
-    <t>13H30</t>
-  </si>
-  <si>
-    <t>HBC AUTION 1</t>
+    <t>TRELAZE HB</t>
+  </si>
+  <si>
+    <t>15H45</t>
+  </si>
+  <si>
+    <t>HBC AUTHION 1</t>
   </si>
   <si>
     <t>BEAUFORT</t>
   </si>
   <si>
-    <t>16H15</t>
-  </si>
-  <si>
-    <t>CS BEAUCOUZE</t>
-  </si>
-  <si>
-    <t>CS LE LION D ANGERS 1</t>
-  </si>
-  <si>
-    <t>LE LION D ANGERS</t>
-  </si>
-  <si>
-    <t>AIZEANY</t>
-  </si>
-  <si>
     <t>14H30</t>
   </si>
   <si>
-    <t>BAUGE</t>
+    <t>Score PDC</t>
+  </si>
+  <si>
+    <t>Score Adv</t>
+  </si>
+  <si>
+    <t>21H</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>JEAN MONNET</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -237,12 +219,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -269,10 +245,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A4ECBB-ED94-404A-B614-82F16F49ED43}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -598,11 +573,11 @@
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -618,8 +593,14 @@
       <c r="E1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -627,17 +608,22 @@
         <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -647,7 +633,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -657,35 +643,27 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -693,45 +671,55 @@
         <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="1">
+        <v>23</v>
+      </c>
+      <c r="G8" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -741,45 +729,29 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>16</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>17</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -787,149 +759,178 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="1">
+        <v>32</v>
+      </c>
+      <c r="G15" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>23</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="F16" s="1">
+        <v>23</v>
+      </c>
+      <c r="G16" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>3</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="F19" s="1">
+        <v>26</v>
+      </c>
+      <c r="G19" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="F20" s="1">
+        <v>28</v>
+      </c>
+      <c r="G20" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="1">
+        <v>16</v>
+      </c>
+      <c r="G21" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -938,29 +939,37 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
       <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>